<commit_message>
arreglo conflicto y arreglo notificaciones
</commit_message>
<xml_diff>
--- a/GrupoSA-web/src/main/webapp/resources/Asistentes.xlsx
+++ b/GrupoSA-web/src/main/webapp/resources/Asistentes.xlsx
@@ -23,16 +23,16 @@
     <t>APELLIDOS</t>
   </si>
   <si>
-    <t>Roberto</t>
+    <t>Eduardo</t>
   </si>
   <si>
-    <t>Ramirez</t>
+    <t>Educado</t>
   </si>
   <si>
-    <t>Miguel</t>
+    <t>Lola</t>
   </si>
   <si>
-    <t>Antonio de la Rosa Santísima</t>
+    <t>Sol</t>
   </si>
 </sst>
 </file>
@@ -96,7 +96,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0</v>
+        <v>103.0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -107,7 +107,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.0</v>
+        <v>105.0</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>